<commit_message>
toolbar and homescreen css
</commit_message>
<xml_diff>
--- a/TutorGroup_Deliverable_5_SprintBacklog.xlsx
+++ b/TutorGroup_Deliverable_5_SprintBacklog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pison\Documents\GitHub\Tutor-Software-Engineering\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hannahyelle/Desktop/Tutor-Software-Engineering/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED424C2-FE55-42A1-BF9E-5EBF5E533352}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{157CBB3E-B098-0E43-BAB6-C016E5587C9F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3540" yWindow="480" windowWidth="26160" windowHeight="17280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
   <si>
     <t>Number</t>
   </si>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t>Chase</t>
+  </si>
+  <si>
+    <t>Hannah - 100%</t>
   </si>
 </sst>
 </file>
@@ -433,19 +436,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1010"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.26953125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="6.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="107.26953125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="107.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24" bestFit="1" customWidth="1"/>
-    <col min="7" max="26" width="10.54296875" customWidth="1"/>
+    <col min="7" max="26" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="42.75" customHeight="1">
@@ -487,7 +490,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" s="9" customFormat="1">
+    <row r="2" spans="1:26" s="9" customFormat="1" ht="16">
       <c r="A2" s="3">
         <v>0</v>
       </c>
@@ -507,7 +510,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:26" s="9" customFormat="1">
+    <row r="3" spans="1:26" s="9" customFormat="1" ht="16">
       <c r="A3" s="3"/>
       <c r="B3" s="10" t="s">
         <v>28</v>
@@ -533,7 +536,7 @@
         <v>3</v>
       </c>
       <c r="E4" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F4" s="4"/>
     </row>
@@ -545,7 +548,9 @@
       <c r="C5" s="7"/>
       <c r="D5" s="5"/>
       <c r="E5" s="7"/>
-      <c r="F5" s="4"/>
+      <c r="F5" s="4" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="6" spans="1:26" ht="27" customHeight="1">
       <c r="A6" s="3"/>

</xml_diff>